<commit_message>
Saving rules for Universal OR strategy
</commit_message>
<xml_diff>
--- a/Order_Management.xlsx
+++ b/Order_Management.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mohammed Khalid\OneDrive\Desktop\WSGTA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mohammed Khalid\OneDrive\Desktop\WSGTA\Github\universal-or-strategy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{270091C7-9991-4D4C-A656-6AE5293B3615}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30D6F581-4B4D-4652-8F4F-95ED29C64246}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{443257C1-151D-4D5B-B416-D4B7290BC384}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="128">
   <si>
     <t>Trade</t>
   </si>
@@ -404,13 +404,28 @@
   </si>
   <si>
     <t xml:space="preserve">Add fibs </t>
+  </si>
+  <si>
+    <t>ORB numbers on chart</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>Click</t>
+  </si>
+  <si>
+    <t>when it goes against auto auto break even</t>
+  </si>
+  <si>
+    <t>Apex Compliance:** Strictly enforce rate limiting (max 1 order modification per second) and risk management rules. Is this in the code now rate limiting?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -471,6 +486,27 @@
     <font>
       <b/>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -640,7 +676,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -656,17 +692,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
@@ -677,9 +707,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1"/>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -693,10 +720,36 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -706,39 +759,38 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="25">
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -965,6 +1017,9 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -1173,20 +1228,20 @@
     <tableColumn id="36" xr3:uid="{2F723897-3760-4B19-AD3B-BCFBA1F3046B}" name="Target 2 " dataDxfId="16"/>
     <tableColumn id="37" xr3:uid="{B0228055-B9F0-4376-9F4B-E5C7ECEC374E}" name="Target 3" dataDxfId="15"/>
     <tableColumn id="17" xr3:uid="{7CC3D155-497E-446B-A522-0C4A9AE7DA8D}" name="BE Trigger" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{5A6E6A7C-0D76-470A-81B6-DC838B39B5C4}" name="BE Offset (t)" dataDxfId="0"/>
-    <tableColumn id="7" xr3:uid="{6FC4F2C6-D6C6-47D3-8D38-72AB148DAFEF}" name="trail1 Trigger (pts)" dataDxfId="13"/>
-    <tableColumn id="16" xr3:uid="{8AA31D74-6B23-44D9-9308-370238BD8AF2}" name="Trail1 Distance (pts)" dataDxfId="12"/>
-    <tableColumn id="18" xr3:uid="{803838AC-CC2F-4B13-BA83-8B235A2B7979}" name="Frequency" dataDxfId="11"/>
-    <tableColumn id="8" xr3:uid="{C8E30A81-9A2B-4FB6-B8DF-121E9D1D8311}" name="Trail2 Trigger (pts)" dataDxfId="10"/>
-    <tableColumn id="15" xr3:uid="{A0CCBB03-A13C-4BC3-9F5E-4DA389FEE99B}" name="Trail2 Distance (pts)" dataDxfId="9"/>
-    <tableColumn id="9" xr3:uid="{005D4A69-D483-4A76-AE2E-EA4663A26F7F}" name="Step 2 Frequency" dataDxfId="8"/>
-    <tableColumn id="14" xr3:uid="{54D8ADB7-AC18-47AE-9CC3-0EB9A0711574}" name="trail3 Trigger (pts)" dataDxfId="7"/>
-    <tableColumn id="19" xr3:uid="{00B2CDE8-9EAA-4C1B-985D-A54CA250F42C}" name="Trail3 Distance (pts)" dataDxfId="6"/>
-    <tableColumn id="20" xr3:uid="{549EE94F-A456-41A9-BD1E-91EF731DFD75}" name="Step 3 Frequency" dataDxfId="5"/>
-    <tableColumn id="35" xr3:uid="{3CC47613-3113-48A8-947D-6BFD5041B252}" name="Direction" dataDxfId="4"/>
-    <tableColumn id="21" xr3:uid="{A81BB64B-3F9E-46D1-8DC6-E7152EFC37AB}" name="Entry Criteria" dataDxfId="3"/>
-    <tableColumn id="22" xr3:uid="{BF3BF641-5A58-4CC8-99E6-52116BA6F0C1}" name="Execution Criteria" dataDxfId="2"/>
-    <tableColumn id="23" xr3:uid="{EDCDBC5F-1F59-4512-81F4-43551DDE86E7}" name="Column1" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{5A6E6A7C-0D76-470A-81B6-DC838B39B5C4}" name="BE Offset (t)" dataDxfId="13"/>
+    <tableColumn id="7" xr3:uid="{6FC4F2C6-D6C6-47D3-8D38-72AB148DAFEF}" name="trail1 Trigger (pts)" dataDxfId="12"/>
+    <tableColumn id="16" xr3:uid="{8AA31D74-6B23-44D9-9308-370238BD8AF2}" name="Trail1 Distance (pts)" dataDxfId="11"/>
+    <tableColumn id="18" xr3:uid="{803838AC-CC2F-4B13-BA83-8B235A2B7979}" name="Frequency" dataDxfId="10"/>
+    <tableColumn id="8" xr3:uid="{C8E30A81-9A2B-4FB6-B8DF-121E9D1D8311}" name="Trail2 Trigger (pts)" dataDxfId="9"/>
+    <tableColumn id="15" xr3:uid="{A0CCBB03-A13C-4BC3-9F5E-4DA389FEE99B}" name="Trail2 Distance (pts)" dataDxfId="8"/>
+    <tableColumn id="9" xr3:uid="{005D4A69-D483-4A76-AE2E-EA4663A26F7F}" name="Step 2 Frequency" dataDxfId="7"/>
+    <tableColumn id="14" xr3:uid="{54D8ADB7-AC18-47AE-9CC3-0EB9A0711574}" name="trail3 Trigger (pts)" dataDxfId="6"/>
+    <tableColumn id="19" xr3:uid="{00B2CDE8-9EAA-4C1B-985D-A54CA250F42C}" name="Trail3 Distance (pts)" dataDxfId="5"/>
+    <tableColumn id="20" xr3:uid="{549EE94F-A456-41A9-BD1E-91EF731DFD75}" name="Step 3 Frequency" dataDxfId="4"/>
+    <tableColumn id="35" xr3:uid="{3CC47613-3113-48A8-947D-6BFD5041B252}" name="Direction" dataDxfId="3"/>
+    <tableColumn id="21" xr3:uid="{A81BB64B-3F9E-46D1-8DC6-E7152EFC37AB}" name="Entry Criteria" dataDxfId="2"/>
+    <tableColumn id="22" xr3:uid="{BF3BF641-5A58-4CC8-99E6-52116BA6F0C1}" name="Execution Criteria" dataDxfId="1"/>
+    <tableColumn id="23" xr3:uid="{EDCDBC5F-1F59-4512-81F4-43551DDE86E7}" name="Column1" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1492,10 +1547,10 @@
   <dimension ref="A1:AL32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="2" ySplit="10" topLeftCell="C20" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="10" topLeftCell="C23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="C27" sqref="C27"/>
+      <selection pane="bottomRight" activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1607,595 +1662,567 @@
       <c r="AK1"/>
       <c r="AL1"/>
     </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    <row r="2" spans="1:38" s="39" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="40" t="s">
         <v>76</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F2" s="40">
         <v>0</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="K2" s="1">
+      <c r="K2" s="40">
         <v>1</v>
       </c>
-      <c r="L2" s="1">
+      <c r="L2" s="40">
         <v>3</v>
       </c>
-      <c r="M2" s="1">
+      <c r="M2" s="40">
         <v>2</v>
       </c>
-      <c r="N2" s="1">
+      <c r="N2" s="40">
         <v>2</v>
       </c>
-      <c r="O2" s="1">
+      <c r="O2" s="40">
         <v>4</v>
       </c>
-      <c r="P2" s="1">
+      <c r="P2" s="40">
         <v>1.5</v>
       </c>
-      <c r="Q2" s="1">
+      <c r="Q2" s="40">
         <v>2</v>
       </c>
-      <c r="R2" s="1">
+      <c r="R2" s="40">
         <v>5</v>
       </c>
-      <c r="S2" s="1">
+      <c r="S2" s="40">
         <v>1</v>
       </c>
-      <c r="T2" s="1">
+      <c r="T2" s="40">
         <v>1</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="U2" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="V2" s="7" t="s">
+      <c r="V2" s="41" t="s">
         <v>90</v>
       </c>
-      <c r="W2" s="1" t="s">
+      <c r="W2" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="X2" s="1" t="s">
+      <c r="X2" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="AI2"/>
-      <c r="AJ2"/>
-      <c r="AK2"/>
-      <c r="AL2"/>
-    </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+    </row>
+    <row r="3" spans="1:38" s="37" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="37" t="s">
         <v>106</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3" s="2">
         <v>0</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="J3" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="K3" s="1">
+      <c r="K3" s="2">
         <v>1</v>
       </c>
-      <c r="L3" s="1">
+      <c r="L3" s="2">
         <v>3</v>
       </c>
-      <c r="M3" s="1">
+      <c r="M3" s="2">
         <v>2</v>
       </c>
-      <c r="N3" s="1">
+      <c r="N3" s="2">
         <v>2</v>
       </c>
-      <c r="O3" s="1">
+      <c r="O3" s="2">
         <v>4</v>
       </c>
-      <c r="P3" s="1">
+      <c r="P3" s="2">
         <v>1.5</v>
       </c>
-      <c r="Q3" s="1">
+      <c r="Q3" s="2">
         <v>2</v>
       </c>
-      <c r="R3" s="1">
+      <c r="R3" s="2">
         <v>5</v>
       </c>
-      <c r="S3" s="1">
+      <c r="S3" s="2">
         <v>1</v>
       </c>
-      <c r="T3" s="1">
+      <c r="T3" s="2">
         <v>1</v>
       </c>
-      <c r="U3" s="1" t="s">
+      <c r="U3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="V3" s="7" t="s">
+      <c r="V3" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="W3" s="1" t="s">
+      <c r="W3" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="X3" s="1" t="s">
+      <c r="X3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="AI3"/>
-      <c r="AJ3"/>
-      <c r="AK3"/>
-      <c r="AL3"/>
-    </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+    </row>
+    <row r="4" spans="1:38" s="42" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="42" t="s">
         <v>101</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="43" t="s">
         <v>57</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4" s="43">
         <v>0</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="43" t="s">
         <v>54</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="I4" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="J4" s="43" t="s">
         <v>54</v>
       </c>
-      <c r="K4" s="1">
+      <c r="K4" s="43">
         <v>1</v>
       </c>
-      <c r="L4" s="1">
+      <c r="L4" s="43">
         <v>3</v>
       </c>
-      <c r="M4" s="1">
+      <c r="M4" s="43">
         <v>2</v>
       </c>
-      <c r="N4" s="1">
+      <c r="N4" s="43">
         <v>2</v>
       </c>
-      <c r="O4" s="1">
+      <c r="O4" s="43">
         <v>4</v>
       </c>
-      <c r="P4" s="1">
+      <c r="P4" s="43">
         <v>1.5</v>
       </c>
-      <c r="Q4" s="1">
+      <c r="Q4" s="43">
         <v>2</v>
       </c>
-      <c r="R4" s="1">
+      <c r="R4" s="43">
         <v>5</v>
       </c>
-      <c r="S4" s="1">
+      <c r="S4" s="43">
         <v>1</v>
       </c>
-      <c r="T4" s="1">
+      <c r="T4" s="43">
         <v>1</v>
       </c>
-      <c r="U4" s="1" t="s">
+      <c r="U4" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="V4" s="7" t="s">
+      <c r="V4" s="44" t="s">
         <v>62</v>
       </c>
-      <c r="W4" s="1" t="s">
+      <c r="W4" s="43" t="s">
         <v>91</v>
       </c>
-      <c r="X4" s="1" t="s">
+      <c r="X4" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="AI4"/>
-      <c r="AJ4"/>
-      <c r="AK4"/>
-      <c r="AL4"/>
-    </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+    </row>
+    <row r="5" spans="1:38" s="34" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="34" t="s">
         <v>104</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5" s="35">
         <v>2</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G5" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="H5" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="I5" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="J5" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="K5" s="1">
+      <c r="K5" s="35">
         <v>1</v>
       </c>
-      <c r="L5" s="1">
+      <c r="L5" s="35">
         <v>3</v>
       </c>
-      <c r="M5" s="1">
+      <c r="M5" s="35">
         <v>2</v>
       </c>
-      <c r="N5" s="1">
+      <c r="N5" s="35">
         <v>2</v>
       </c>
-      <c r="O5" s="1">
+      <c r="O5" s="35">
         <v>4</v>
       </c>
-      <c r="P5" s="1">
+      <c r="P5" s="35">
         <v>1.5</v>
       </c>
-      <c r="Q5" s="1">
+      <c r="Q5" s="35">
         <v>2</v>
       </c>
-      <c r="R5" s="1">
+      <c r="R5" s="35">
         <v>5</v>
       </c>
-      <c r="S5" s="1">
+      <c r="S5" s="35">
         <v>1</v>
       </c>
-      <c r="T5" s="1">
+      <c r="T5" s="35">
         <v>1</v>
       </c>
-      <c r="U5" s="1" t="s">
+      <c r="U5" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="V5" s="7" t="s">
+      <c r="V5" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="W5" s="1" t="s">
+      <c r="W5" s="35" t="s">
         <v>88</v>
       </c>
-      <c r="X5" s="1" t="s">
+      <c r="X5" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="AI5"/>
-      <c r="AJ5"/>
-      <c r="AK5"/>
-      <c r="AL5"/>
-    </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+    </row>
+    <row r="6" spans="1:38" s="37" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="45" t="s">
         <v>103</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="37" t="s">
         <v>102</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="2">
         <v>0</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G6" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H6" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="I6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="J6" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="K6" s="1">
+      <c r="K6" s="2">
         <v>1</v>
       </c>
-      <c r="L6" s="1">
+      <c r="L6" s="2">
         <v>3</v>
       </c>
-      <c r="M6" s="1">
+      <c r="M6" s="2">
         <v>2</v>
       </c>
-      <c r="N6" s="1">
+      <c r="N6" s="2">
         <v>2</v>
       </c>
-      <c r="O6" s="1">
+      <c r="O6" s="2">
         <v>4</v>
       </c>
-      <c r="P6" s="1">
+      <c r="P6" s="2">
         <v>1.5</v>
       </c>
-      <c r="Q6" s="1">
+      <c r="Q6" s="2">
         <v>2</v>
       </c>
-      <c r="R6" s="1">
+      <c r="R6" s="2">
         <v>5</v>
       </c>
-      <c r="S6" s="1">
+      <c r="S6" s="2">
         <v>1</v>
       </c>
-      <c r="T6" s="1">
+      <c r="T6" s="2">
         <v>1</v>
       </c>
-      <c r="U6" s="1" t="s">
+      <c r="U6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="V6" s="7" t="s">
+      <c r="V6" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="W6" s="1" t="s">
+      <c r="W6" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="X6" s="1" t="s">
+      <c r="X6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="AI6"/>
-      <c r="AJ6"/>
-      <c r="AK6"/>
-      <c r="AL6"/>
-    </row>
-    <row r="7" spans="1:38" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="8" t="s">
+    </row>
+    <row r="7" spans="1:38" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="F7" s="9">
+      <c r="F7" s="8">
         <v>3</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="G7" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="H7" s="9" t="s">
+      <c r="H7" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="I7" s="9" t="s">
+      <c r="I7" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="J7" s="9" t="s">
+      <c r="J7" s="8" t="s">
         <v>52</v>
       </c>
       <c r="K7" s="1">
         <v>1</v>
       </c>
-      <c r="L7" s="9">
+      <c r="L7" s="8">
         <v>3</v>
       </c>
-      <c r="M7" s="9">
+      <c r="M7" s="8">
         <v>2</v>
       </c>
-      <c r="N7" s="9">
+      <c r="N7" s="8">
         <v>2</v>
       </c>
-      <c r="O7" s="9">
+      <c r="O7" s="8">
         <v>4</v>
       </c>
-      <c r="P7" s="9">
+      <c r="P7" s="8">
         <v>1.5</v>
       </c>
-      <c r="Q7" s="9">
+      <c r="Q7" s="8">
         <v>2</v>
       </c>
-      <c r="R7" s="9">
+      <c r="R7" s="8">
         <v>5</v>
       </c>
-      <c r="S7" s="9">
+      <c r="S7" s="8">
         <v>1</v>
       </c>
-      <c r="T7" s="9">
+      <c r="T7" s="8">
         <v>1</v>
       </c>
-      <c r="U7" s="9" t="s">
+      <c r="U7" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="V7" s="10" t="s">
+      <c r="V7" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="W7" s="9" t="s">
+      <c r="W7" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="X7" s="9" t="s">
+      <c r="X7" s="8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:38" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+    <row r="8" spans="1:38" s="39" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="39" t="s">
         <v>59</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="40" t="s">
         <v>75</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8" s="40">
         <v>0</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G8" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="H8" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="I8" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="J8" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="K8" s="1">
+      <c r="K8" s="40">
         <v>1</v>
       </c>
-      <c r="L8" s="1">
+      <c r="L8" s="40">
         <v>3</v>
       </c>
-      <c r="M8" s="1">
+      <c r="M8" s="40">
         <v>2</v>
       </c>
-      <c r="N8" s="1">
+      <c r="N8" s="40">
         <v>2</v>
       </c>
-      <c r="O8" s="1">
+      <c r="O8" s="40">
         <v>4</v>
       </c>
-      <c r="P8" s="1">
+      <c r="P8" s="40">
         <v>1.5</v>
       </c>
-      <c r="Q8" s="1">
+      <c r="Q8" s="40">
         <v>2</v>
       </c>
-      <c r="R8" s="1">
+      <c r="R8" s="40">
         <v>5</v>
       </c>
-      <c r="S8" s="1">
+      <c r="S8" s="40">
         <v>1</v>
       </c>
-      <c r="T8" s="1">
+      <c r="T8" s="40">
         <v>1</v>
       </c>
-      <c r="U8" s="1" t="s">
+      <c r="U8" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="V8" s="7" t="s">
+      <c r="V8" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="W8" s="1" t="s">
+      <c r="W8" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="X8" s="1" t="s">
+      <c r="X8" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="AI8"/>
-      <c r="AJ8"/>
-      <c r="AK8"/>
-      <c r="AL8"/>
-    </row>
-    <row r="9" spans="1:38" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+    </row>
+    <row r="9" spans="1:38" s="37" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F9" s="2">
         <v>0</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="G9" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="H9" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="I9" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="J9" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="K9" s="1">
+      <c r="K9" s="2">
         <v>1</v>
       </c>
-      <c r="L9" s="1">
+      <c r="L9" s="2">
         <v>3</v>
       </c>
-      <c r="M9" s="1">
+      <c r="M9" s="2">
         <v>2</v>
       </c>
-      <c r="N9" s="1">
+      <c r="N9" s="2">
         <v>2</v>
       </c>
-      <c r="O9" s="1">
+      <c r="O9" s="2">
         <v>4</v>
       </c>
-      <c r="P9" s="1">
+      <c r="P9" s="2">
         <v>1.5</v>
       </c>
-      <c r="Q9" s="1">
+      <c r="Q9" s="2">
         <v>2</v>
       </c>
-      <c r="R9" s="1">
+      <c r="R9" s="2">
         <v>5</v>
       </c>
-      <c r="S9" s="1">
+      <c r="S9" s="2">
         <v>1</v>
       </c>
-      <c r="T9" s="1">
+      <c r="T9" s="2">
         <v>1</v>
       </c>
-      <c r="U9" s="1" t="s">
+      <c r="U9" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="V9" s="7" t="s">
+      <c r="V9" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="W9" s="1" t="s">
+      <c r="W9" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="X9" s="1" t="s">
+      <c r="X9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="AI9"/>
-      <c r="AJ9"/>
-      <c r="AK9"/>
-      <c r="AL9"/>
     </row>
     <row r="13" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
@@ -2261,13 +2288,24 @@
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>123</v>
+      </c>
       <c r="C26" t="s">
         <v>122</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C27" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="6" t="s">
         <v>69</v>
+      </c>
+      <c r="C28" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
@@ -2352,231 +2390,220 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A37874B-405E-42F6-A097-C7A8365BB04E}">
-  <dimension ref="A1:F50"/>
+  <dimension ref="A1:E50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="49.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9" style="17" customWidth="1"/>
-    <col min="3" max="3" width="9.36328125" style="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.36328125" customWidth="1"/>
-    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" style="15" customWidth="1"/>
+    <col min="3" max="3" width="9.36328125" style="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="20" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:5" ht="20" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="28" t="s">
         <v>93</v>
       </c>
-      <c r="C1" s="25"/>
-    </row>
-    <row r="2" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="13" t="s">
+      <c r="C1" s="28"/>
+      <c r="D1" s="21" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="22" t="s">
         <v>99</v>
       </c>
-      <c r="C4" s="30" t="s">
+      <c r="C4" s="23" t="s">
         <v>98</v>
       </c>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-    </row>
-    <row r="5" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="13" t="s">
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+    </row>
+    <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="32"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="13"/>
-      <c r="B6" s="22"/>
-      <c r="C6" s="22"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-    </row>
-    <row r="7" spans="1:6" s="12" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="13"/>
-      <c r="B7" s="22"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="13" t="s">
+      <c r="C5" s="30"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="11"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+    </row>
+    <row r="7" spans="1:5" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="11"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="29" t="s">
+      <c r="B8" s="22" t="s">
         <v>96</v>
       </c>
-      <c r="C8" s="30" t="s">
+      <c r="C8" s="23" t="s">
         <v>97</v>
       </c>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" s="13" t="s">
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="B9" s="33" t="s">
+      <c r="B9" s="24" t="s">
         <v>96</v>
       </c>
-      <c r="C9" s="34" t="s">
+      <c r="C9" s="25" t="s">
         <v>97</v>
       </c>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-    </row>
-    <row r="10" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="13" t="s">
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+    </row>
+    <row r="10" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="35" t="s">
+      <c r="B10" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="C10" s="36" t="s">
+      <c r="C10" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="14"/>
-      <c r="B11" s="28"/>
-      <c r="C11" s="28"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" s="14"/>
-      <c r="B12" s="23"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" s="13" t="s">
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="12"/>
+      <c r="B11" s="33"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" s="12"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="27" t="s">
+      <c r="B13" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="27"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" s="15" t="s">
+      <c r="C13" s="32"/>
+      <c r="D13" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="E13" s="14"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="27" t="s">
+      <c r="B14" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="C14" s="27"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" s="15" t="s">
+      <c r="C14" s="32"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B15" s="20">
+      <c r="B15" s="17">
         <v>9</v>
       </c>
-      <c r="C15" s="20">
+      <c r="C15" s="17">
         <v>15</v>
       </c>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" s="13" t="s">
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="20" t="s">
+      <c r="B16" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="C16" s="21" t="s">
+      <c r="C16" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A17" s="15" t="s">
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="20" t="s">
+      <c r="B17" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="C17" s="21" t="s">
+      <c r="C17" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A18" s="13"/>
-      <c r="B18" s="26" t="s">
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" s="11"/>
+      <c r="B18" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="C18" s="26"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C18" s="31"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="6" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>36</v>
       </c>

</xml_diff>

<commit_message>
Button Rows and Trend Trade
</commit_message>
<xml_diff>
--- a/Order_Management.xlsx
+++ b/Order_Management.xlsx
@@ -8,14 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mohammed Khalid\OneDrive\Desktop\WSGTA\Github\universal-or-strategy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCFFC627-9AED-4DF0-B95E-EA10D42FBB9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F477B251-F757-48BA-BDCD-6BCF41C605A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{443257C1-151D-4D5B-B416-D4B7290BC384}"/>
   </bookViews>
   <sheets>
     <sheet name="MES &amp; MGC" sheetId="1" r:id="rId1"/>
-    <sheet name="Design1" sheetId="7" r:id="rId2"/>
-    <sheet name="Design2" sheetId="8" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="68">
   <si>
     <t>Trade</t>
   </si>
@@ -80,18 +78,9 @@
     <t>Market</t>
   </si>
   <si>
-    <t>ORB MOMO</t>
-  </si>
-  <si>
     <t>Break of the 5 min then the 15 min opening range</t>
   </si>
   <si>
-    <t>Retest of the 5 min then the 15 min opening range</t>
-  </si>
-  <si>
-    <t>RMA</t>
-  </si>
-  <si>
     <t>Reversal inside the 5 min then the 15 min opening range</t>
   </si>
   <si>
@@ -128,24 +117,9 @@
     <t>10 point move</t>
   </si>
   <si>
-    <t>BOX</t>
-  </si>
-  <si>
-    <t>ORB MIDWAY</t>
-  </si>
-  <si>
-    <t>ORB LOW</t>
-  </si>
-  <si>
-    <t>ORB HIGH</t>
-  </si>
-  <si>
     <t>Entry Type</t>
   </si>
   <si>
-    <t>FLATTEN</t>
-  </si>
-  <si>
     <t>1 x ATR</t>
   </si>
   <si>
@@ -170,18 +144,9 @@
     <t>Entry Buffer (t)</t>
   </si>
   <si>
-    <t>FFMA</t>
-  </si>
-  <si>
     <t>Stop Loss</t>
   </si>
   <si>
-    <t>4 pts trail of 9 ema once over 9 ema</t>
-  </si>
-  <si>
-    <t>4 pts trail of entry ema</t>
-  </si>
-  <si>
     <t>trail1 Trigger (pts)</t>
   </si>
   <si>
@@ -212,27 +177,6 @@
     <t>30 EMA, 65 EMA, 200 EMA, PIVOT POINT or VWAP</t>
   </si>
   <si>
-    <t>Buttons</t>
-  </si>
-  <si>
-    <t>DB</t>
-  </si>
-  <si>
-    <t>DT</t>
-  </si>
-  <si>
-    <t>BUY</t>
-  </si>
-  <si>
-    <t>SELL</t>
-  </si>
-  <si>
-    <t>SELL LOW</t>
-  </si>
-  <si>
-    <t>BUY HIGH</t>
-  </si>
-  <si>
     <t>No restriction on number of entries</t>
   </si>
   <si>
@@ -263,48 +207,6 @@
     <t>Trail2 Trigger (pts)</t>
   </si>
   <si>
-    <t xml:space="preserve">ORB MOMO BOX </t>
-  </si>
-  <si>
-    <t>TREND</t>
-  </si>
-  <si>
-    <t>DBDT</t>
-  </si>
-  <si>
-    <t>T1</t>
-  </si>
-  <si>
-    <t>T2</t>
-  </si>
-  <si>
-    <t>RUNNER</t>
-  </si>
-  <si>
-    <t>BE</t>
-  </si>
-  <si>
-    <t>FLAT</t>
-  </si>
-  <si>
-    <t>MOMO</t>
-  </si>
-  <si>
-    <t>MID</t>
-  </si>
-  <si>
-    <t>LOW</t>
-  </si>
-  <si>
-    <t>TOP</t>
-  </si>
-  <si>
-    <t>ACTIONS (DROP DOWN MENU)</t>
-  </si>
-  <si>
-    <t>BREAK</t>
-  </si>
-  <si>
     <t>Target 4</t>
   </si>
   <si>
@@ -326,35 +228,23 @@
     <t>OR Inside Reversal (RMA)</t>
   </si>
   <si>
-    <t>LONG</t>
-  </si>
-  <si>
-    <t>SHORT</t>
-  </si>
-  <si>
-    <t>BOX IS LONG AND SHORT THE OR BREAK</t>
-  </si>
-  <si>
-    <t>TRADES (DROP DOWN MENU)</t>
-  </si>
-  <si>
-    <t>UI</t>
-  </si>
-  <si>
-    <t>T3</t>
-  </si>
-  <si>
     <t>.5 x atr</t>
   </si>
   <si>
     <t>.5 point or .5 x ATR</t>
+  </si>
+  <si>
+    <t>1.1 x ATR trail of 9 ema once over 9 ema</t>
+  </si>
+  <si>
+    <t>9 ema entry starts with 2 pts stop then 1.1 x ATR trail of entry ema when price is above or below in my favor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -384,14 +274,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFC00000"/>
       <name val="Calibri"/>
@@ -404,39 +286,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFF00"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF0070C0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="14">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -449,74 +300,8 @@
         <bgColor theme="4"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF6699FF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor theme="4" tint="0.79998168889431442"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC00000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF7030A0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="1"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="11">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -535,105 +320,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </top>
-      <bottom style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -650,103 +341,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="7" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="26">
@@ -1510,10 +1117,10 @@
   <dimension ref="A1:AN9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="2" ySplit="10" topLeftCell="D11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="10" topLeftCell="E11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="A14" sqref="A14"/>
+      <selection pane="bottomRight" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1553,67 +1160,67 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>92</v>
+        <v>60</v>
       </c>
       <c r="C1" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>91</v>
+        <v>59</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>90</v>
+        <v>58</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>89</v>
+        <v>57</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>73</v>
+        <v>55</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>74</v>
+        <v>56</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="W1" s="3" t="s">
         <v>1</v>
@@ -1638,7 +1245,7 @@
         <v>9</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>47</v>
+        <v>67</v>
       </c>
       <c r="F2" s="1">
         <v>0</v>
@@ -1647,16 +1254,16 @@
         <v>1</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="L2" s="1">
         <v>1</v>
@@ -1689,13 +1296,13 @@
         <v>1</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="W2" s="5" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="X2" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="Y2" s="1" t="s">
         <v>10</v>
@@ -1711,13 +1318,13 @@
         <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>93</v>
+        <v>61</v>
       </c>
       <c r="F3" s="1">
         <v>0</v>
@@ -1726,16 +1333,16 @@
         <v>1</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="L3" s="1">
         <v>1</v>
@@ -1768,13 +1375,13 @@
         <v>1</v>
       </c>
       <c r="V3" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="W3" s="5" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="X3" s="1" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="Y3" s="1" t="s">
         <v>10</v>
@@ -1790,13 +1397,13 @@
         <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="F4" s="1">
         <v>0</v>
@@ -1805,16 +1412,16 @@
         <v>1</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="L4" s="1">
         <v>1</v>
@@ -1847,13 +1454,13 @@
         <v>1</v>
       </c>
       <c r="V4" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="W4" s="5" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="X4" s="1" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="Y4" s="1" t="s">
         <v>10</v>
@@ -1866,19 +1473,19 @@
     </row>
     <row r="5" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="C5" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>8</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>103</v>
+        <v>65</v>
       </c>
       <c r="F5" s="1">
         <v>2</v>
@@ -1887,16 +1494,16 @@
         <v>1</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="L5" s="1">
         <v>1</v>
@@ -1929,13 +1536,13 @@
         <v>1</v>
       </c>
       <c r="V5" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="W5" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="X5" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="X5" s="1" t="s">
-        <v>53</v>
       </c>
       <c r="Y5" s="1" t="s">
         <v>10</v>
@@ -1948,19 +1555,19 @@
     </row>
     <row r="6" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" s="19" t="s">
-        <v>67</v>
+        <v>20</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>49</v>
       </c>
       <c r="C6" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>93</v>
+        <v>61</v>
       </c>
       <c r="F6" s="1">
         <v>0</v>
@@ -1969,16 +1576,16 @@
         <v>1</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="L6" s="1">
         <v>1</v>
@@ -2011,13 +1618,13 @@
         <v>1</v>
       </c>
       <c r="V6" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="W6" s="5" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="X6" s="1" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="Y6" s="1" t="s">
         <v>10</v>
@@ -2030,13 +1637,13 @@
     </row>
     <row r="7" spans="1:40" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
-        <v>94</v>
+        <v>62</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>8</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>102</v>
+        <v>64</v>
       </c>
       <c r="F7" s="7">
         <v>3</v>
@@ -2045,16 +1652,16 @@
         <v>1</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="K7" s="7" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="L7" s="1">
         <v>1</v>
@@ -2087,13 +1694,13 @@
         <v>1</v>
       </c>
       <c r="V7" s="7" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="W7" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="X7" s="7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="Y7" s="7" t="s">
         <v>10</v>
@@ -2101,13 +1708,13 @@
     </row>
     <row r="8" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>46</v>
+        <v>66</v>
       </c>
       <c r="F8" s="1">
         <v>0</v>
@@ -2116,16 +1723,16 @@
         <v>1</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="L8" s="1">
         <v>1</v>
@@ -2158,13 +1765,13 @@
         <v>1</v>
       </c>
       <c r="V8" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="W8" s="5" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="X8" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="Y8" s="1" t="s">
         <v>10</v>
@@ -2177,13 +1784,13 @@
     </row>
     <row r="9" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>95</v>
+        <v>63</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>93</v>
+        <v>61</v>
       </c>
       <c r="F9" s="1">
         <v>0</v>
@@ -2192,16 +1799,16 @@
         <v>1</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="L9" s="1">
         <v>1</v>
@@ -2234,13 +1841,13 @@
         <v>1</v>
       </c>
       <c r="V9" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="W9" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="X9" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="Y9" s="1" t="s">
         <v>10</v>
@@ -2309,334 +1916,4 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A37874B-405E-42F6-A097-C7A8365BB04E}">
-  <dimension ref="A1:H8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="49.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.1796875" style="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.54296875" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="7.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="36.90625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" ht="20" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="41" t="s">
-        <v>100</v>
-      </c>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="40" t="s">
-        <v>71</v>
-      </c>
-      <c r="H1" s="40"/>
-    </row>
-    <row r="2" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="11"/>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="11"/>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="B4" s="35" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="37" t="s">
-        <v>44</v>
-      </c>
-      <c r="D4" s="34" t="s">
-        <v>76</v>
-      </c>
-      <c r="E4" s="35" t="s">
-        <v>77</v>
-      </c>
-      <c r="F4" s="33" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="B5" s="33" t="s">
-        <v>88</v>
-      </c>
-      <c r="C5" s="34" t="s">
-        <v>86</v>
-      </c>
-      <c r="D5" s="35" t="s">
-        <v>84</v>
-      </c>
-      <c r="E5" s="35" t="s">
-        <v>85</v>
-      </c>
-      <c r="F5" s="42" t="s">
-        <v>30</v>
-      </c>
-      <c r="G5" s="27" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="B6" s="33" t="s">
-        <v>88</v>
-      </c>
-      <c r="C6" s="34" t="s">
-        <v>86</v>
-      </c>
-      <c r="D6" s="35" t="s">
-        <v>84</v>
-      </c>
-      <c r="E6" s="35" t="s">
-        <v>85</v>
-      </c>
-      <c r="F6" s="42"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="B7" s="30" t="s">
-        <v>78</v>
-      </c>
-      <c r="C7" s="30" t="s">
-        <v>79</v>
-      </c>
-      <c r="D7" s="30" t="s">
-        <v>101</v>
-      </c>
-      <c r="E7" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="F7" s="29" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" s="38"/>
-      <c r="B8" s="39">
-        <v>0.25</v>
-      </c>
-      <c r="C8" s="39">
-        <v>0.5</v>
-      </c>
-      <c r="D8" s="39">
-        <v>0.75</v>
-      </c>
-      <c r="E8" s="39">
-        <v>1</v>
-      </c>
-      <c r="F8" s="28" t="s">
-        <v>82</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="F5:F6"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88F3901F-17EB-43B8-B8B9-79E2CAA76DC0}">
-  <dimension ref="A1:C18"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:3" ht="20" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="40" t="s">
-        <v>58</v>
-      </c>
-      <c r="C1" s="40"/>
-    </row>
-    <row r="2" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-    </row>
-    <row r="3" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="C4" s="21" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="B5" s="43" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" s="44"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="10"/>
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
-    </row>
-    <row r="7" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="10"/>
-      <c r="B7" s="17"/>
-      <c r="C7" s="17"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B8" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="C8" s="21" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="B9" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="C9" s="23" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" s="24" t="s">
-        <v>61</v>
-      </c>
-      <c r="C10" s="25" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" s="11"/>
-      <c r="B11" s="45"/>
-      <c r="C11" s="45"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" s="11"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="18"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="26" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" s="26"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="46" t="s">
-        <v>44</v>
-      </c>
-      <c r="C14" s="46"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" s="15">
-        <v>9</v>
-      </c>
-      <c r="C15" s="15">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="B16" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="B17" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="C17" s="16" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" s="10"/>
-      <c r="B18" s="47" t="s">
-        <v>35</v>
-      </c>
-      <c r="C18" s="47"/>
-    </row>
-  </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B18:C18"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
attempted to bring back live numbers rtd
</commit_message>
<xml_diff>
--- a/Order_Management.xlsx
+++ b/Order_Management.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mohammed Khalid\OneDrive\Desktop\WSGTA\Github\universal-or-strategy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{168AA415-FEE8-42E1-9680-284CF42A5756}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C7C53BB-9A00-4961-AD3B-B9C4B0CB0D61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{443257C1-151D-4D5B-B416-D4B7290BC384}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="70">
   <si>
     <t>Trade</t>
   </si>
@@ -238,6 +238,12 @@
   </si>
   <si>
     <t>.5 point</t>
+  </si>
+  <si>
+    <t>Max Stop Loss</t>
+  </si>
+  <si>
+    <t>Min Stop Loss</t>
   </si>
 </sst>
 </file>
@@ -356,7 +362,13 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="26">
+  <dxfs count="28">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -786,34 +798,36 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71F716AF-2BD1-48E3-89E2-7887C18BCD1C}" name="Table3" displayName="Table3" ref="A1:Y9" totalsRowShown="0" dataDxfId="25">
-  <autoFilter ref="A1:Y9" xr:uid="{71F716AF-2BD1-48E3-89E2-7887C18BCD1C}"/>
-  <tableColumns count="25">
-    <tableColumn id="1" xr3:uid="{F1231F65-FE9D-4F05-9AEA-375A9B44E98F}" name="Trade" dataDxfId="24"/>
-    <tableColumn id="13" xr3:uid="{0729B735-1C69-4AA6-BA5D-11E984B423C0}" name="Entry Type" dataDxfId="23"/>
-    <tableColumn id="12" xr3:uid="{DF4C2B2A-2C13-4816-A984-7C0F07631786}" name="Stop Loss" dataDxfId="22"/>
-    <tableColumn id="34" xr3:uid="{F9532B55-F96A-49FA-BEC8-315BE26D9EF5}" name="Entry Buffer (t)" dataDxfId="21"/>
-    <tableColumn id="3" xr3:uid="{A2225BB0-4217-4042-8E71-A7CC1BAD5016}" name="Target1 (pts) " dataDxfId="20"/>
-    <tableColumn id="4" xr3:uid="{BDD4D5EF-A942-40E7-AA6B-847C848BBE45}" name="Target 2 " dataDxfId="19"/>
-    <tableColumn id="36" xr3:uid="{2F723897-3760-4B19-AD3B-BCFBA1F3046B}" name="Target 3 " dataDxfId="18"/>
-    <tableColumn id="37" xr3:uid="{B0228055-B9F0-4376-9F4B-E5C7ECEC374E}" name="Target 4" dataDxfId="17"/>
-    <tableColumn id="17" xr3:uid="{7CC3D155-497E-446B-A522-0C4A9AE7DA8D}" name="BE Trigger" dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{5A6E6A7C-0D76-470A-81B6-DC838B39B5C4}" name="BE Offset (t)" dataDxfId="15"/>
-    <tableColumn id="7" xr3:uid="{6FC4F2C6-D6C6-47D3-8D38-72AB148DAFEF}" name="trail1 Trigger (pts)" dataDxfId="14"/>
-    <tableColumn id="16" xr3:uid="{8AA31D74-6B23-44D9-9308-370238BD8AF2}" name="Trail1 Distance (pts)" dataDxfId="13"/>
-    <tableColumn id="18" xr3:uid="{803838AC-CC2F-4B13-BA83-8B235A2B7979}" name="Frequency" dataDxfId="12"/>
-    <tableColumn id="8" xr3:uid="{C8E30A81-9A2B-4FB6-B8DF-121E9D1D8311}" name="Trail2 Trigger (pts)" dataDxfId="11"/>
-    <tableColumn id="15" xr3:uid="{A0CCBB03-A13C-4BC3-9F5E-4DA389FEE99B}" name="Trail2 Distance (pts)" dataDxfId="10"/>
-    <tableColumn id="9" xr3:uid="{005D4A69-D483-4A76-AE2E-EA4663A26F7F}" name="Step 2 Frequency" dataDxfId="9"/>
-    <tableColumn id="14" xr3:uid="{54D8ADB7-AC18-47AE-9CC3-0EB9A0711574}" name="trail3 Trigger (pts)" dataDxfId="8"/>
-    <tableColumn id="19" xr3:uid="{00B2CDE8-9EAA-4C1B-985D-A54CA250F42C}" name="Trail3 Distance (pts)" dataDxfId="7"/>
-    <tableColumn id="20" xr3:uid="{549EE94F-A456-41A9-BD1E-91EF731DFD75}" name="Step 3 Frequency" dataDxfId="6"/>
-    <tableColumn id="35" xr3:uid="{3CC47613-3113-48A8-947D-6BFD5041B252}" name="Direction" dataDxfId="5"/>
-    <tableColumn id="21" xr3:uid="{A81BB64B-3F9E-46D1-8DC6-E7152EFC37AB}" name="Entry Criteria" dataDxfId="4"/>
-    <tableColumn id="22" xr3:uid="{BF3BF641-5A58-4CC8-99E6-52116BA6F0C1}" name="Execution Criteria" dataDxfId="3"/>
-    <tableColumn id="23" xr3:uid="{EDCDBC5F-1F59-4512-81F4-43551DDE86E7}" name="Column1" dataDxfId="2"/>
-    <tableColumn id="26" xr3:uid="{956D6271-21DD-4ECC-845E-606737643F42}" name="Target Profit target per trade" dataDxfId="1"/>
-    <tableColumn id="25" xr3:uid="{8CDF4F04-3F12-4C6E-9874-3AFD2217F0C1}" name="Notes" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71F716AF-2BD1-48E3-89E2-7887C18BCD1C}" name="Table3" displayName="Table3" ref="A1:AA9" totalsRowShown="0" dataDxfId="27">
+  <autoFilter ref="A1:AA9" xr:uid="{71F716AF-2BD1-48E3-89E2-7887C18BCD1C}"/>
+  <tableColumns count="27">
+    <tableColumn id="1" xr3:uid="{F1231F65-FE9D-4F05-9AEA-375A9B44E98F}" name="Trade" dataDxfId="26"/>
+    <tableColumn id="13" xr3:uid="{0729B735-1C69-4AA6-BA5D-11E984B423C0}" name="Entry Type" dataDxfId="25"/>
+    <tableColumn id="12" xr3:uid="{DF4C2B2A-2C13-4816-A984-7C0F07631786}" name="Stop Loss" dataDxfId="24"/>
+    <tableColumn id="6" xr3:uid="{68703295-41BB-4627-A11C-79FAC734FF2E}" name="Min Stop Loss" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{0AA803B7-A230-425D-9987-28DA65718CCE}" name="Max Stop Loss" dataDxfId="1"/>
+    <tableColumn id="34" xr3:uid="{F9532B55-F96A-49FA-BEC8-315BE26D9EF5}" name="Entry Buffer (t)" dataDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{A2225BB0-4217-4042-8E71-A7CC1BAD5016}" name="Target1 (pts) " dataDxfId="22"/>
+    <tableColumn id="4" xr3:uid="{BDD4D5EF-A942-40E7-AA6B-847C848BBE45}" name="Target 2 " dataDxfId="21"/>
+    <tableColumn id="36" xr3:uid="{2F723897-3760-4B19-AD3B-BCFBA1F3046B}" name="Target 3 " dataDxfId="20"/>
+    <tableColumn id="37" xr3:uid="{B0228055-B9F0-4376-9F4B-E5C7ECEC374E}" name="Target 4" dataDxfId="19"/>
+    <tableColumn id="17" xr3:uid="{7CC3D155-497E-446B-A522-0C4A9AE7DA8D}" name="BE Trigger" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{5A6E6A7C-0D76-470A-81B6-DC838B39B5C4}" name="BE Offset (t)" dataDxfId="17"/>
+    <tableColumn id="7" xr3:uid="{6FC4F2C6-D6C6-47D3-8D38-72AB148DAFEF}" name="trail1 Trigger (pts)" dataDxfId="16"/>
+    <tableColumn id="16" xr3:uid="{8AA31D74-6B23-44D9-9308-370238BD8AF2}" name="Trail1 Distance (pts)" dataDxfId="15"/>
+    <tableColumn id="18" xr3:uid="{803838AC-CC2F-4B13-BA83-8B235A2B7979}" name="Frequency" dataDxfId="14"/>
+    <tableColumn id="8" xr3:uid="{C8E30A81-9A2B-4FB6-B8DF-121E9D1D8311}" name="Trail2 Trigger (pts)" dataDxfId="13"/>
+    <tableColumn id="15" xr3:uid="{A0CCBB03-A13C-4BC3-9F5E-4DA389FEE99B}" name="Trail2 Distance (pts)" dataDxfId="12"/>
+    <tableColumn id="9" xr3:uid="{005D4A69-D483-4A76-AE2E-EA4663A26F7F}" name="Step 2 Frequency" dataDxfId="11"/>
+    <tableColumn id="14" xr3:uid="{54D8ADB7-AC18-47AE-9CC3-0EB9A0711574}" name="trail3 Trigger (pts)" dataDxfId="10"/>
+    <tableColumn id="19" xr3:uid="{00B2CDE8-9EAA-4C1B-985D-A54CA250F42C}" name="Trail3 Distance (pts)" dataDxfId="9"/>
+    <tableColumn id="20" xr3:uid="{549EE94F-A456-41A9-BD1E-91EF731DFD75}" name="Step 3 Frequency" dataDxfId="8"/>
+    <tableColumn id="35" xr3:uid="{3CC47613-3113-48A8-947D-6BFD5041B252}" name="Direction" dataDxfId="7"/>
+    <tableColumn id="21" xr3:uid="{A81BB64B-3F9E-46D1-8DC6-E7152EFC37AB}" name="Entry Criteria" dataDxfId="6"/>
+    <tableColumn id="22" xr3:uid="{BF3BF641-5A58-4CC8-99E6-52116BA6F0C1}" name="Execution Criteria" dataDxfId="5"/>
+    <tableColumn id="23" xr3:uid="{EDCDBC5F-1F59-4512-81F4-43551DDE86E7}" name="Column1" dataDxfId="4"/>
+    <tableColumn id="26" xr3:uid="{956D6271-21DD-4ECC-845E-606737643F42}" name="Target Profit target per trade" dataDxfId="3"/>
+    <tableColumn id="25" xr3:uid="{8CDF4F04-3F12-4C6E-9874-3AFD2217F0C1}" name="Notes" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1116,10 +1130,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C7E259D-8BC0-4231-80EC-F205308B971F}">
-  <dimension ref="A1:AP9"/>
+  <dimension ref="A1:AR9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D2" sqref="D2:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1127,38 +1141,40 @@
     <col min="1" max="1" width="30.36328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.26953125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="92" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.6328125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.1796875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="22.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="20.36328125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="22.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="19.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="48.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="137.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="27.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="66.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11.1796875" customWidth="1"/>
-    <col min="27" max="27" width="28.453125" customWidth="1"/>
-    <col min="28" max="28" width="8.90625" style="1" customWidth="1"/>
-    <col min="39" max="39" width="8.7265625" style="1"/>
-    <col min="40" max="40" width="18.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.6328125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.1796875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="22.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="20.36328125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="22.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="48.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="137.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="27.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="66.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="11.1796875" customWidth="1"/>
+    <col min="29" max="29" width="28.453125" customWidth="1"/>
+    <col min="30" max="30" width="8.90625" style="1" customWidth="1"/>
     <col min="41" max="41" width="8.7265625" style="1"/>
-    <col min="42" max="42" width="19.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="18.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="8.7265625" style="1"/>
+    <col min="44" max="44" width="19.54296875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1169,78 +1185,84 @@
         <v>36</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="U1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="V1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="W1" s="1" t="s">
+      <c r="W1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="X1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Z1" t="s">
         <v>60</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AA1" t="s">
         <v>53</v>
       </c>
-      <c r="AB1"/>
-      <c r="AM1"/>
-      <c r="AN1"/>
+      <c r="AD1"/>
       <c r="AO1"/>
       <c r="AP1"/>
+      <c r="AQ1"/>
+      <c r="AR1"/>
     </row>
-    <row r="2" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1251,74 +1273,80 @@
         <v>66</v>
       </c>
       <c r="D2" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1">
+        <v>8</v>
+      </c>
+      <c r="F2" s="1">
         <v>0</v>
       </c>
-      <c r="E2" s="1">
-        <v>1</v>
-      </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1">
+        <v>1</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="J2" s="1">
-        <v>1</v>
-      </c>
-      <c r="K2" s="1">
+      <c r="L2" s="1">
+        <v>1</v>
+      </c>
+      <c r="M2" s="1">
         <v>3</v>
       </c>
-      <c r="L2" s="1">
-        <v>2</v>
-      </c>
-      <c r="M2" s="1">
-        <v>2</v>
-      </c>
       <c r="N2" s="1">
+        <v>2</v>
+      </c>
+      <c r="O2" s="1">
+        <v>2</v>
+      </c>
+      <c r="P2" s="1">
         <v>4</v>
       </c>
-      <c r="O2" s="1">
+      <c r="Q2" s="1">
         <v>1.5</v>
       </c>
-      <c r="P2" s="1">
-        <v>2</v>
-      </c>
-      <c r="Q2" s="1">
+      <c r="R2" s="1">
+        <v>2</v>
+      </c>
+      <c r="S2" s="1">
         <v>5</v>
       </c>
-      <c r="R2" s="1">
-        <v>1</v>
-      </c>
-      <c r="S2" s="1">
-        <v>1</v>
-      </c>
-      <c r="T2" s="1" t="s">
+      <c r="T2" s="1">
+        <v>1</v>
+      </c>
+      <c r="U2" s="1">
+        <v>1</v>
+      </c>
+      <c r="V2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="U2" s="5" t="s">
+      <c r="W2" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="V2" s="1" t="s">
+      <c r="X2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="W2" s="1" t="s">
+      <c r="Y2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="X2"/>
-      <c r="Y2"/>
-      <c r="AB2"/>
-      <c r="AM2"/>
-      <c r="AN2"/>
+      <c r="Z2"/>
+      <c r="AA2"/>
+      <c r="AD2"/>
       <c r="AO2"/>
       <c r="AP2"/>
+      <c r="AQ2"/>
+      <c r="AR2"/>
     </row>
-    <row r="3" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -1329,76 +1357,82 @@
         <v>61</v>
       </c>
       <c r="D3" s="1">
+        <v>3</v>
+      </c>
+      <c r="E3" s="1">
+        <v>8</v>
+      </c>
+      <c r="F3" s="1">
         <v>0</v>
       </c>
-      <c r="E3" s="1">
-        <v>1</v>
-      </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1">
+        <v>1</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="J3" s="1">
-        <v>1</v>
-      </c>
-      <c r="K3" s="1">
+      <c r="L3" s="1">
+        <v>1</v>
+      </c>
+      <c r="M3" s="1">
         <v>3</v>
       </c>
-      <c r="L3" s="1">
-        <v>2</v>
-      </c>
-      <c r="M3" s="1">
-        <v>2</v>
-      </c>
       <c r="N3" s="1">
+        <v>2</v>
+      </c>
+      <c r="O3" s="1">
+        <v>2</v>
+      </c>
+      <c r="P3" s="1">
         <v>4</v>
       </c>
-      <c r="O3" s="1">
+      <c r="Q3" s="1">
         <v>1.5</v>
       </c>
-      <c r="P3" s="1">
-        <v>2</v>
-      </c>
-      <c r="Q3" s="1">
+      <c r="R3" s="1">
+        <v>2</v>
+      </c>
+      <c r="S3" s="1">
         <v>5</v>
       </c>
-      <c r="R3" s="1">
-        <v>1</v>
-      </c>
-      <c r="S3" s="1">
-        <v>1</v>
-      </c>
-      <c r="T3" s="1" t="s">
+      <c r="T3" s="1">
+        <v>1</v>
+      </c>
+      <c r="U3" s="1">
+        <v>1</v>
+      </c>
+      <c r="V3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="U3" s="5" t="s">
+      <c r="W3" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="V3" s="1" t="s">
+      <c r="X3" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="W3" s="1" t="s">
+      <c r="Y3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="X3"/>
-      <c r="Y3" t="s">
+      <c r="Z3"/>
+      <c r="AA3" t="s">
         <v>52</v>
       </c>
-      <c r="AB3"/>
-      <c r="AM3"/>
-      <c r="AN3"/>
+      <c r="AD3"/>
       <c r="AO3"/>
       <c r="AP3"/>
+      <c r="AQ3"/>
+      <c r="AR3"/>
     </row>
-    <row r="4" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -1409,76 +1443,82 @@
         <v>31</v>
       </c>
       <c r="D4" s="1">
+        <v>3</v>
+      </c>
+      <c r="E4" s="1">
+        <v>8</v>
+      </c>
+      <c r="F4" s="1">
         <v>0</v>
       </c>
-      <c r="E4" s="1">
-        <v>1</v>
-      </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1">
+        <v>1</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="J4" s="1">
-        <v>1</v>
-      </c>
-      <c r="K4" s="1">
+      <c r="L4" s="1">
+        <v>1</v>
+      </c>
+      <c r="M4" s="1">
         <v>3</v>
       </c>
-      <c r="L4" s="1">
-        <v>2</v>
-      </c>
-      <c r="M4" s="1">
-        <v>2</v>
-      </c>
       <c r="N4" s="1">
+        <v>2</v>
+      </c>
+      <c r="O4" s="1">
+        <v>2</v>
+      </c>
+      <c r="P4" s="1">
         <v>4</v>
       </c>
-      <c r="O4" s="1">
+      <c r="Q4" s="1">
         <v>1.5</v>
       </c>
-      <c r="P4" s="1">
-        <v>2</v>
-      </c>
-      <c r="Q4" s="1">
+      <c r="R4" s="1">
+        <v>2</v>
+      </c>
+      <c r="S4" s="1">
         <v>5</v>
       </c>
-      <c r="R4" s="1">
-        <v>1</v>
-      </c>
-      <c r="S4" s="1">
-        <v>1</v>
-      </c>
-      <c r="T4" s="1" t="s">
+      <c r="T4" s="1">
+        <v>1</v>
+      </c>
+      <c r="U4" s="1">
+        <v>1</v>
+      </c>
+      <c r="V4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="U4" s="5" t="s">
+      <c r="W4" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="V4" s="1" t="s">
+      <c r="X4" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="W4" s="1" t="s">
+      <c r="Y4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="X4"/>
-      <c r="Y4" t="s">
+      <c r="Z4"/>
+      <c r="AA4" t="s">
         <v>47</v>
       </c>
-      <c r="AB4"/>
-      <c r="AM4"/>
-      <c r="AN4"/>
+      <c r="AD4"/>
       <c r="AO4"/>
       <c r="AP4"/>
+      <c r="AQ4"/>
+      <c r="AR4"/>
     </row>
-    <row r="5" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -1489,78 +1529,84 @@
         <v>67</v>
       </c>
       <c r="D5" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E5" s="1">
-        <v>1</v>
-      </c>
-      <c r="F5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="1">
+        <v>2</v>
+      </c>
+      <c r="G5" s="1">
+        <v>1</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="K5" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="J5" s="1">
-        <v>1</v>
-      </c>
-      <c r="K5" s="1">
+      <c r="L5" s="1">
+        <v>1</v>
+      </c>
+      <c r="M5" s="1">
         <v>3</v>
       </c>
-      <c r="L5" s="1">
-        <v>2</v>
-      </c>
-      <c r="M5" s="1">
-        <v>2</v>
-      </c>
       <c r="N5" s="1">
+        <v>2</v>
+      </c>
+      <c r="O5" s="1">
+        <v>2</v>
+      </c>
+      <c r="P5" s="1">
         <v>4</v>
       </c>
-      <c r="O5" s="1">
+      <c r="Q5" s="1">
         <v>1.5</v>
       </c>
-      <c r="P5" s="1">
-        <v>2</v>
-      </c>
-      <c r="Q5" s="1">
+      <c r="R5" s="1">
+        <v>2</v>
+      </c>
+      <c r="S5" s="1">
         <v>5</v>
       </c>
-      <c r="R5" s="1">
-        <v>1</v>
-      </c>
-      <c r="S5" s="1">
-        <v>1</v>
-      </c>
-      <c r="T5" s="1" t="s">
+      <c r="T5" s="1">
+        <v>1</v>
+      </c>
+      <c r="U5" s="1">
+        <v>1</v>
+      </c>
+      <c r="V5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="U5" s="5" t="s">
+      <c r="W5" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="V5" s="1" t="s">
+      <c r="X5" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="W5" s="1" t="s">
+      <c r="Y5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="X5" t="s">
+      <c r="Z5" t="s">
         <v>51</v>
       </c>
-      <c r="Y5" t="s">
+      <c r="AA5" t="s">
         <v>50</v>
       </c>
-      <c r="AB5"/>
-      <c r="AM5"/>
-      <c r="AN5"/>
+      <c r="AD5"/>
       <c r="AO5"/>
       <c r="AP5"/>
+      <c r="AQ5"/>
+      <c r="AR5"/>
     </row>
-    <row r="6" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -1571,78 +1617,84 @@
         <v>61</v>
       </c>
       <c r="D6" s="1">
+        <v>3</v>
+      </c>
+      <c r="E6" s="1">
+        <v>8</v>
+      </c>
+      <c r="F6" s="1">
         <v>0</v>
       </c>
-      <c r="E6" s="1">
-        <v>1</v>
-      </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1">
+        <v>1</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="I6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="K6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="J6" s="1">
-        <v>1</v>
-      </c>
-      <c r="K6" s="1">
+      <c r="L6" s="1">
+        <v>1</v>
+      </c>
+      <c r="M6" s="1">
         <v>3</v>
       </c>
-      <c r="L6" s="1">
-        <v>2</v>
-      </c>
-      <c r="M6" s="1">
-        <v>2</v>
-      </c>
       <c r="N6" s="1">
+        <v>2</v>
+      </c>
+      <c r="O6" s="1">
+        <v>2</v>
+      </c>
+      <c r="P6" s="1">
         <v>4</v>
       </c>
-      <c r="O6" s="1">
+      <c r="Q6" s="1">
         <v>1.5</v>
       </c>
-      <c r="P6" s="1">
-        <v>2</v>
-      </c>
-      <c r="Q6" s="1">
+      <c r="R6" s="1">
+        <v>2</v>
+      </c>
+      <c r="S6" s="1">
         <v>5</v>
       </c>
-      <c r="R6" s="1">
-        <v>1</v>
-      </c>
-      <c r="S6" s="1">
-        <v>1</v>
-      </c>
-      <c r="T6" s="1" t="s">
+      <c r="T6" s="1">
+        <v>1</v>
+      </c>
+      <c r="U6" s="1">
+        <v>1</v>
+      </c>
+      <c r="V6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="U6" s="5" t="s">
+      <c r="W6" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="V6" s="1" t="s">
+      <c r="X6" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="W6" s="1" t="s">
+      <c r="Y6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="X6" s="10" t="s">
+      <c r="Z6" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="Y6" t="s">
+      <c r="AA6" t="s">
         <v>48</v>
       </c>
-      <c r="AB6"/>
-      <c r="AM6"/>
-      <c r="AN6"/>
+      <c r="AD6"/>
       <c r="AO6"/>
       <c r="AP6"/>
+      <c r="AQ6"/>
+      <c r="AR6"/>
     </row>
-    <row r="7" spans="1:42" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:44" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
         <v>62</v>
       </c>
@@ -1652,68 +1704,74 @@
       <c r="C7" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="1">
         <v>3</v>
       </c>
       <c r="E7" s="1">
-        <v>1</v>
-      </c>
-      <c r="F7" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="7">
+        <v>3</v>
+      </c>
+      <c r="G7" s="1">
+        <v>1</v>
+      </c>
+      <c r="H7" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="I7" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H7" s="7" t="s">
+      <c r="J7" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="I7" s="7" t="s">
+      <c r="K7" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="J7" s="1">
-        <v>1</v>
-      </c>
-      <c r="K7" s="7">
+      <c r="L7" s="1">
+        <v>1</v>
+      </c>
+      <c r="M7" s="7">
         <v>3</v>
       </c>
-      <c r="L7" s="7">
-        <v>2</v>
-      </c>
-      <c r="M7" s="7">
-        <v>2</v>
-      </c>
       <c r="N7" s="7">
+        <v>2</v>
+      </c>
+      <c r="O7" s="7">
+        <v>2</v>
+      </c>
+      <c r="P7" s="7">
         <v>4</v>
       </c>
-      <c r="O7" s="7">
+      <c r="Q7" s="7">
         <v>1.5</v>
       </c>
-      <c r="P7" s="7">
-        <v>2</v>
-      </c>
-      <c r="Q7" s="7">
+      <c r="R7" s="7">
+        <v>2</v>
+      </c>
+      <c r="S7" s="7">
         <v>5</v>
       </c>
-      <c r="R7" s="7">
-        <v>1</v>
-      </c>
-      <c r="S7" s="7">
-        <v>1</v>
-      </c>
-      <c r="T7" s="7" t="s">
+      <c r="T7" s="7">
+        <v>1</v>
+      </c>
+      <c r="U7" s="7">
+        <v>1</v>
+      </c>
+      <c r="V7" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="U7" s="8" t="s">
+      <c r="W7" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="V7" s="7" t="s">
+      <c r="X7" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="W7" s="7" t="s">
+      <c r="Y7" s="7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>32</v>
       </c>
@@ -1724,74 +1782,80 @@
         <v>65</v>
       </c>
       <c r="D8" s="1">
+        <v>3</v>
+      </c>
+      <c r="E8" s="1">
+        <v>8</v>
+      </c>
+      <c r="F8" s="1">
         <v>0</v>
       </c>
-      <c r="E8" s="1">
-        <v>1</v>
-      </c>
-      <c r="F8" s="1" t="s">
+      <c r="G8" s="1">
+        <v>1</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="I8" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="J8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="K8" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="J8" s="1">
-        <v>1</v>
-      </c>
-      <c r="K8" s="1">
+      <c r="L8" s="1">
+        <v>1</v>
+      </c>
+      <c r="M8" s="1">
         <v>3</v>
       </c>
-      <c r="L8" s="1">
-        <v>2</v>
-      </c>
-      <c r="M8" s="1">
-        <v>2</v>
-      </c>
       <c r="N8" s="1">
+        <v>2</v>
+      </c>
+      <c r="O8" s="1">
+        <v>2</v>
+      </c>
+      <c r="P8" s="1">
         <v>4</v>
       </c>
-      <c r="O8" s="1">
+      <c r="Q8" s="1">
         <v>1.5</v>
       </c>
-      <c r="P8" s="1">
-        <v>2</v>
-      </c>
-      <c r="Q8" s="1">
+      <c r="R8" s="1">
+        <v>2</v>
+      </c>
+      <c r="S8" s="1">
         <v>5</v>
       </c>
-      <c r="R8" s="1">
-        <v>1</v>
-      </c>
-      <c r="S8" s="1">
-        <v>1</v>
-      </c>
-      <c r="T8" s="1" t="s">
+      <c r="T8" s="1">
+        <v>1</v>
+      </c>
+      <c r="U8" s="1">
+        <v>1</v>
+      </c>
+      <c r="V8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="U8" s="5" t="s">
+      <c r="W8" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="V8" s="1" t="s">
+      <c r="X8" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="W8" s="1" t="s">
+      <c r="Y8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="X8"/>
-      <c r="Y8"/>
-      <c r="AB8"/>
-      <c r="AM8"/>
-      <c r="AN8"/>
+      <c r="Z8"/>
+      <c r="AA8"/>
+      <c r="AD8"/>
       <c r="AO8"/>
       <c r="AP8"/>
+      <c r="AQ8"/>
+      <c r="AR8"/>
     </row>
-    <row r="9" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>63</v>
       </c>
@@ -1802,76 +1866,82 @@
         <v>61</v>
       </c>
       <c r="D9" s="1">
+        <v>3</v>
+      </c>
+      <c r="E9" s="1">
+        <v>8</v>
+      </c>
+      <c r="F9" s="1">
         <v>0</v>
       </c>
-      <c r="E9" s="1">
-        <v>1</v>
-      </c>
-      <c r="F9" s="1" t="s">
+      <c r="G9" s="1">
+        <v>1</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="I9" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="J9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="K9" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="J9" s="1">
-        <v>1</v>
-      </c>
-      <c r="K9" s="1">
+      <c r="L9" s="1">
+        <v>1</v>
+      </c>
+      <c r="M9" s="1">
         <v>3</v>
       </c>
-      <c r="L9" s="1">
-        <v>2</v>
-      </c>
-      <c r="M9" s="1">
-        <v>2</v>
-      </c>
       <c r="N9" s="1">
+        <v>2</v>
+      </c>
+      <c r="O9" s="1">
+        <v>2</v>
+      </c>
+      <c r="P9" s="1">
         <v>4</v>
       </c>
-      <c r="O9" s="1">
+      <c r="Q9" s="1">
         <v>1.5</v>
       </c>
-      <c r="P9" s="1">
-        <v>2</v>
-      </c>
-      <c r="Q9" s="1">
+      <c r="R9" s="1">
+        <v>2</v>
+      </c>
+      <c r="S9" s="1">
         <v>5</v>
       </c>
-      <c r="R9" s="1">
-        <v>1</v>
-      </c>
-      <c r="S9" s="1">
-        <v>1</v>
-      </c>
-      <c r="T9" s="1" t="s">
+      <c r="T9" s="1">
+        <v>1</v>
+      </c>
+      <c r="U9" s="1">
+        <v>1</v>
+      </c>
+      <c r="V9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="U9" s="5" t="s">
+      <c r="W9" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="V9" s="1" t="s">
+      <c r="X9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="W9" s="1" t="s">
+      <c r="Y9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="X9"/>
-      <c r="Y9"/>
-      <c r="AB9"/>
-      <c r="AM9"/>
-      <c r="AN9"/>
+      <c r="Z9"/>
+      <c r="AA9"/>
+      <c r="AD9"/>
       <c r="AO9"/>
       <c r="AP9"/>
+      <c r="AQ9"/>
+      <c r="AR9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="A1:S9 X1:Y9">
+  <conditionalFormatting sqref="Z1:AA9 A1:U9">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -1883,7 +1953,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:Y9">
+  <conditionalFormatting sqref="A1:AA9">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>